<commit_message>
first results android emulator
</commit_message>
<xml_diff>
--- a/Data/emulatorChoice/Averages.xlsx
+++ b/Data/emulatorChoice/Averages.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Camille FOURNIER\Documents\Scripts\Data\emulatorChoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{9B204872-0F1B-47D5-BD4C-511269D0B62E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482A940A-F7F0-4C20-B941-3785E864CD8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="46695" yWindow="7575" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Real" sheetId="1" r:id="rId1"/>
     <sheet name="Genymotion" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
@@ -35,11 +35,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Requête - galaxyS6_70_geny_910" description="Connexion à la requête « galaxyS6_70_geny_910 » dans le classeur." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Requête - galaxyS6_70_geny_910" description="Connexion à la requête « galaxyS6_70_geny_910 » dans le classeur." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=galaxyS6_70_geny_910;Extended Properties=&quot;&quot;" command="SELECT * FROM [galaxyS6_70_geny_910]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Requête - galaxyS6_70_real_910" description="Connexion à la requête « galaxyS6_70_real_910 » dans le classeur." type="5" refreshedVersion="6" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Requête - galaxyS6_70_real_910" description="Connexion à la requête « galaxyS6_70_real_910 » dans le classeur." type="5" refreshedVersion="6" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=galaxyS6_70_real_910;Extended Properties=&quot;&quot;" command="SELECT * FROM [galaxyS6_70_real_910]"/>
   </connection>
 </connections>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DonnéesExternes_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DonnéesExternes_1" connectionId="1" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7" unboundColumnsRight="1">
     <queryTableFields count="6">
       <queryTableField id="1" name="Clock" tableColumnId="1"/>
@@ -218,15 +218,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="galaxyS6_70_geny_910" displayName="galaxyS6_70_geny_910" ref="A1:F122" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F122"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="galaxyS6_70_geny_910" displayName="galaxyS6_70_geny_910" ref="A1:F122" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F122" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" uniqueName="1" name="Clock" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name=" Total frames rendered" queryTableFieldId="2"/>
-    <tableColumn id="3" uniqueName="3" name=" Janky frames" queryTableFieldId="3"/>
-    <tableColumn id="4" uniqueName="4" name=" CPU%" queryTableFieldId="4"/>
-    <tableColumn id="5" uniqueName="5" name=" PSS " queryTableFieldId="5"/>
-    <tableColumn id="6" uniqueName="6" name="FPS" queryTableFieldId="6" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="Clock" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name=" Total frames rendered" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name=" Janky frames" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name=" CPU%" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name=" PSS " queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="FPS" queryTableFieldId="6" dataDxfId="0">
       <calculatedColumnFormula>(1-galaxyS6_70_geny_910[[#This Row],[ Janky frames]]/galaxyS6_70_geny_910[[#This Row],[ Total frames rendered]])*60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -530,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,10 +3108,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>

</xml_diff>